<commit_message>
Update Excel SCD0011 until SCD0016
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0010-115 -Penyesuaian Kriteria Account Plan SRM.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0010-115 -Penyesuaian Kriteria Account Plan SRM.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9069A3D0-C49D-4654-A327-EB7617E568BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A5C3B5-63C5-4F8B-8D7D-8A9060B6E310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SCD0167" sheetId="2" r:id="rId1"/>
+    <sheet name="SCD0010" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -93,9 +93,6 @@
  Expired usulan Approval : Tanggal 25 bulan November 2021 jam 23:59 WIB</t>
   </si>
   <si>
-    <t>DGS-182</t>
-  </si>
-  <si>
     <t>Penyesuaian Kriteria Account Plan secara Umum (Sesuai pada BSDD 2.10) : SRM, SRM Growth, SRM Hunter</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Rinjani</t>
+  </si>
+  <si>
+    <t>SCD0010-115</t>
   </si>
 </sst>
 </file>
@@ -530,14 +530,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
@@ -610,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>21</v>
@@ -628,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>13</v>
@@ -637,7 +637,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>15</v>
@@ -659,13 +659,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>21</v>
@@ -677,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>13</v>
@@ -686,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>15</v>

</xml_diff>